<commit_message>
1. Migrated to Net 6.0 2. Removed support for Framework 4.52 as this is long dead and near impossible to maintain support for now 3. Set cell formatting to accounting for row 3 in SH151-Custom-Cell-Currency.xlsx to resolve negative/positive return value inconsistency with non-numerical values.
</commit_message>
<xml_diff>
--- a/TestFiles/SH151-Custom-Cell-Format-Currency.xlsx
+++ b/TestFiles/SH151-Custom-Cell-Format-Currency.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,15 +20,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="8">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="168" formatCode="_ [$CHF-100C]\ * #,##0.00_ ;_ [$CHF-100C]\ * \-#,##0.00_ ;_ [$CHF-100C]\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="169" formatCode="_-[$₩-412]* #,##0.00_-;\-[$₩-412]* #,##0.00_-;_-[$₩-412]* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="_-[$£-809]* #,##0.00_-;[Red]\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+  <numFmts count="9">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="169" formatCode="_ [$CHF-100C]\ * #,##0.00_ ;_ [$CHF-100C]\ * \-#,##0.00_ ;_ [$CHF-100C]\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="170" formatCode="_-[$₩-412]* #,##0.00_-;\-[$₩-412]* #,##0.00_-;_-[$₩-412]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="171" formatCode="_-[$£-809]* #,##0.00_-;[Red]\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -65,18 +66,19 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -361,12 +363,12 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="13.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1">
         <v>123.45</v>
       </c>
@@ -392,7 +394,7 @@
         <v>123.45</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>-123.45</v>
       </c>
@@ -418,11 +420,11 @@
         <v>-123.45</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>0</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="9">
         <v>0</v>
       </c>
       <c r="C3" s="3">

</xml_diff>